<commit_message>
some changes were made
</commit_message>
<xml_diff>
--- a/source code/Final draft/the material sizes.xlsx
+++ b/source code/Final draft/the material sizes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\desktop D\3rd year\PUSL3190_MDCGunathilaka\diagrams\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\desktop D\3rd year\PUSL3190_MDCGunathilaka\source code\Final draft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764E7E58-7E85-48AE-B21A-D14968BDE76B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F83E61-F624-4416-B8C6-7B260262F44D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="2490" windowWidth="24240" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cotton" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="28">
   <si>
     <t>(one)</t>
   </si>
@@ -321,7 +321,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -448,11 +448,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -511,6 +522,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -875,8 +889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6:I9"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1100,10 +1114,10 @@
       <c r="U6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="V6" s="22"/>
-      <c r="W6" s="22" t="s">
-        <v>25</v>
-      </c>
+      <c r="V6" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="W6" s="22"/>
       <c r="X6" s="22"/>
       <c r="Y6" s="22"/>
       <c r="Z6" s="22"/>
@@ -1128,7 +1142,7 @@
       </c>
       <c r="V7" s="21"/>
       <c r="W7" s="21"/>
-      <c r="X7" s="21"/>
+      <c r="X7" s="28"/>
       <c r="Y7" s="21"/>
       <c r="Z7" s="21"/>
       <c r="AA7" s="21"/>
@@ -1168,9 +1182,6 @@
       </c>
       <c r="V8" s="22"/>
       <c r="W8" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="X8" s="22" t="s">
         <v>25</v>
       </c>
       <c r="Y8" s="22"/>
@@ -1297,10 +1308,10 @@
       <c r="V12" s="22"/>
       <c r="W12" s="22"/>
       <c r="X12" s="22"/>
-      <c r="Y12" s="22"/>
-      <c r="Z12" s="22" t="s">
-        <v>25</v>
-      </c>
+      <c r="Y12" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z12" s="22"/>
       <c r="AA12" s="22"/>
       <c r="AB12" s="8"/>
     </row>

</xml_diff>